<commit_message>
Updated function with current car values
</commit_message>
<xml_diff>
--- a/driver.xlsx
+++ b/driver.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tim Kogucki\github\Quarter-Car-Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{838B2140-7ADD-48D8-BF9D-6C7FBCEE7F7C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{136B53B9-9BE1-41A8-B17A-3A9641B870A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="15" windowWidth="2430" windowHeight="11835" activeTab="1" xr2:uid="{1ABFF8E3-CBCC-421F-80B2-B6B72DA4F2D9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{1ABFF8E3-CBCC-421F-80B2-B6B72DA4F2D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Driver" sheetId="1" r:id="rId1"/>
-    <sheet name="Low" sheetId="2" r:id="rId2"/>
-    <sheet name="High" sheetId="3" r:id="rId3"/>
+    <sheet name="High_Adj" sheetId="2" r:id="rId2"/>
+    <sheet name="Low_Adj" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -79,13 +80,13 @@
     <t>lb</t>
   </si>
   <si>
-    <t>Low</t>
-  </si>
-  <si>
     <t>Speed</t>
   </si>
   <si>
     <t>Force</t>
+  </si>
+  <si>
+    <t>High_Adj</t>
   </si>
 </sst>
 </file>
@@ -439,18 +440,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C97356C9-EE27-4399-837F-C91C8FB76048}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -461,7 +462,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -472,7 +473,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -483,7 +484,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -494,23 +495,23 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -521,7 +522,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -532,7 +533,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -543,7 +544,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -561,28 +562,60 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B021BE45-AC28-4542-B627-66B7694582AA}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2">
         <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>0.5</v>
+      </c>
+      <c r="B3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>2.25</v>
+      </c>
+      <c r="B4">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -592,28 +625,52 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74335640-F8AC-4332-81CB-326264A2A6B0}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2">
         <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
found sign error causing weird behaviour
</commit_message>
<xml_diff>
--- a/driver.xlsx
+++ b/driver.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tim Kogucki\github\Quarter-Car-Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{136B53B9-9BE1-41A8-B17A-3A9641B870A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71354685-FC15-4878-BC26-F328F452FD8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{1ABFF8E3-CBCC-421F-80B2-B6B72DA4F2D9}"/>
+    <workbookView xWindow="15060" yWindow="9885" windowWidth="12150" windowHeight="6495" activeTab="1" xr2:uid="{1ABFF8E3-CBCC-421F-80B2-B6B72DA4F2D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Driver" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,6 @@
     <sheet name="Low_Adj" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -440,18 +439,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C97356C9-EE27-4399-837F-C91C8FB76048}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -462,7 +461,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -473,7 +472,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -484,7 +483,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -495,7 +494,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -503,7 +502,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -511,7 +510,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -522,7 +521,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -533,7 +532,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -544,7 +543,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -564,13 +563,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B021BE45-AC28-4542-B627-66B7694582AA}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -578,7 +577,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -586,7 +585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0.5</v>
       </c>
@@ -594,7 +593,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2.25</v>
       </c>
@@ -602,7 +601,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -610,7 +609,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>8</v>
       </c>
@@ -631,9 +630,9 @@
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -641,7 +640,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -649,7 +648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5</v>
       </c>
@@ -657,7 +656,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>8</v>
       </c>
@@ -665,7 +664,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Update with ride and pitch study
</commit_message>
<xml_diff>
--- a/driver.xlsx
+++ b/driver.xlsx
@@ -1,23 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tim Kogucki\github\Quarter-Car-Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71354685-FC15-4878-BC26-F328F452FD8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F50D711-243D-435A-B28D-8AF656A7832E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15060" yWindow="9885" windowWidth="12150" windowHeight="6495" activeTab="1" xr2:uid="{1ABFF8E3-CBCC-421F-80B2-B6B72DA4F2D9}"/>
+    <workbookView xWindow="20310" yWindow="3675" windowWidth="5745" windowHeight="6495" activeTab="3" xr2:uid="{1ABFF8E3-CBCC-421F-80B2-B6B72DA4F2D9}"/>
   </bookViews>
   <sheets>
-    <sheet name="Driver" sheetId="1" r:id="rId1"/>
-    <sheet name="High_Adj" sheetId="2" r:id="rId2"/>
-    <sheet name="Low_Adj" sheetId="3" r:id="rId3"/>
+    <sheet name="Simulation" sheetId="4" r:id="rId1"/>
+    <sheet name="Vehicle_Param" sheetId="1" r:id="rId2"/>
+    <sheet name="High_Adj" sheetId="2" r:id="rId3"/>
+    <sheet name="Low_Adj" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
   <si>
     <t>Value</t>
   </si>
@@ -86,13 +88,34 @@
   </si>
   <si>
     <t>High_Adj</t>
+  </si>
+  <si>
+    <t>Rear Motion Ratio</t>
+  </si>
+  <si>
+    <t>Front Motion Ratio</t>
+  </si>
+  <si>
+    <t>Vehicle Speed</t>
+  </si>
+  <si>
+    <t>Step Input Height</t>
+  </si>
+  <si>
+    <t>mph</t>
+  </si>
+  <si>
+    <t>in</t>
+  </si>
+  <si>
+    <t>Tire Radius</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -100,16 +123,43 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -117,14 +167,68 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
+    <cellStyle name="20% - Accent2" xfId="2" builtinId="34"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -436,11 +540,74 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C97356C9-EE27-4399-837F-C91C8FB76048}">
-  <dimension ref="A1:C10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5BBB9AD-1D44-4D73-886E-8FE06192CB4F}">
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="2">
+        <v>60</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="2">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C97356C9-EE27-4399-837F-C91C8FB76048}">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -450,172 +617,129 @@
     <col min="3" max="3" width="5.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>560</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>400</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>450</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>20</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>21</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <v>135.19999999999999</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
         <v>177.8</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B021BE45-AC28-4542-B627-66B7694582AA}">
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>0.5</v>
-      </c>
-      <c r="B3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2.25</v>
-      </c>
-      <c r="B4">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>8</v>
-      </c>
-      <c r="B6">
-        <v>155</v>
-      </c>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C12" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -623,20 +747,83 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74335640-F8AC-4332-81CB-326264A2A6B0}">
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B021BE45-AC28-4542-B627-66B7694582AA}">
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0.5</v>
+      </c>
+      <c r="B3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2.25</v>
+      </c>
+      <c r="B4">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>155</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74335640-F8AC-4332-81CB-326264A2A6B0}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>